<commit_message>
fix calculations and data scaling
</commit_message>
<xml_diff>
--- a/data/dispersion.xlsx
+++ b/data/dispersion.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadi.bessudo/Library/CloudStorage/GoogleDrive-gadibessudo@gmail.com/My Drive/Projects/University/Lab C/2025a/WaveParticleDuality/wave-particle-duality-experiment-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F6FFC0-AADF-5544-A4F6-9028593B480D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0FC11E-2091-7140-9F95-77B0E186DA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{1B13B885-15DB-B340-AE80-EE0D226B88C8}"/>
   </bookViews>
   <sheets>
     <sheet name="dispersion" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,28 +476,28 @@
         <v>4.2</v>
       </c>
       <c r="B2">
-        <v>2.6</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>4.7</v>
+        <v>47</v>
       </c>
       <c r="E2">
-        <v>5.3</v>
+        <v>53</v>
       </c>
       <c r="F2">
-        <v>2.2999999999999998</v>
+        <v>23</v>
       </c>
       <c r="G2">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="H2">
-        <v>4.0999999999999996</v>
+        <v>41</v>
       </c>
       <c r="I2">
-        <v>4.7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -505,28 +505,28 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2.7</v>
+        <v>27</v>
       </c>
       <c r="C3">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>4.8</v>
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>5.6</v>
+        <v>56</v>
       </c>
       <c r="F3">
-        <v>2.2999999999999998</v>
+        <v>23</v>
       </c>
       <c r="G3">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="H3">
-        <v>4.2</v>
+        <v>42</v>
       </c>
       <c r="I3">
-        <v>4.9000000000000004</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -534,28 +534,28 @@
         <v>3.8</v>
       </c>
       <c r="B4">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="D4">
-        <v>4.9000000000000004</v>
+        <v>49</v>
       </c>
       <c r="E4">
-        <v>5.6</v>
+        <v>56</v>
       </c>
       <c r="F4">
-        <v>2.4</v>
+        <v>24</v>
       </c>
       <c r="G4">
-        <v>2.9</v>
+        <v>29</v>
       </c>
       <c r="H4">
-        <v>4.4000000000000004</v>
+        <v>44</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -563,28 +563,28 @@
         <v>3.6</v>
       </c>
       <c r="B5">
-        <v>2.7</v>
+        <v>27</v>
       </c>
       <c r="C5">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="D5">
-        <v>4.9000000000000004</v>
+        <v>49</v>
       </c>
       <c r="E5">
-        <v>5.7</v>
+        <v>57</v>
       </c>
       <c r="F5">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="G5">
-        <v>3.1</v>
+        <v>31</v>
       </c>
       <c r="H5">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="I5">
-        <v>5.3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -592,28 +592,28 @@
         <v>3.4</v>
       </c>
       <c r="B6">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>5.7</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>2.7</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="H6">
-        <v>4.7</v>
+        <v>47</v>
       </c>
       <c r="I6">
-        <v>5.5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -621,28 +621,28 @@
         <v>3.2</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>3.4</v>
+        <v>34</v>
       </c>
       <c r="D7">
-        <v>5.0999999999999996</v>
+        <v>51</v>
       </c>
       <c r="E7">
-        <v>5.9</v>
+        <v>59</v>
       </c>
       <c r="F7">
-        <v>2.6</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="H7">
-        <v>4.8</v>
+        <v>48</v>
       </c>
       <c r="I7">
-        <v>5.6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -650,28 +650,28 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>3.6</v>
+        <v>36</v>
       </c>
       <c r="D8">
-        <v>5.4</v>
+        <v>54</v>
       </c>
       <c r="E8">
-        <v>6.3</v>
+        <v>63</v>
       </c>
       <c r="F8">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="G8">
-        <v>3.4</v>
+        <v>34</v>
       </c>
       <c r="H8">
-        <v>4.9000000000000004</v>
+        <v>49</v>
       </c>
       <c r="I8">
-        <v>5.9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -679,28 +679,28 @@
         <v>2.8</v>
       </c>
       <c r="B9">
-        <v>3.1</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>3.7</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>5.5</v>
+        <v>55</v>
       </c>
       <c r="E9">
-        <v>6.4</v>
+        <v>64</v>
       </c>
       <c r="F9">
-        <v>2.9</v>
+        <v>29</v>
       </c>
       <c r="G9">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="H9">
-        <v>5.2</v>
+        <v>52</v>
       </c>
       <c r="I9">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -708,28 +708,28 @@
         <v>2.6</v>
       </c>
       <c r="B10">
-        <v>3.4</v>
+        <v>34</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>5.9</v>
+        <v>59</v>
       </c>
       <c r="E10">
-        <v>6.7</v>
+        <v>67</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G10">
-        <v>3.6</v>
+        <v>36</v>
       </c>
       <c r="H10">
-        <v>5.5</v>
+        <v>55</v>
       </c>
       <c r="I10">
-        <v>6.4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -737,28 +737,28 @@
         <v>2.4</v>
       </c>
       <c r="B11">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>4.0999999999999996</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>5.6</v>
+        <v>56</v>
       </c>
       <c r="E11">
-        <v>6.8</v>
+        <v>68</v>
       </c>
       <c r="F11">
-        <v>3.1</v>
+        <v>31</v>
       </c>
       <c r="G11">
-        <v>3.8</v>
+        <v>38</v>
       </c>
       <c r="H11">
-        <v>5.7</v>
+        <v>57</v>
       </c>
       <c r="I11">
-        <v>6.6</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -766,28 +766,28 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B12">
-        <v>3.4</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>4.2</v>
+        <v>42</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="E12">
-        <v>7.1</v>
+        <v>71</v>
       </c>
       <c r="F12">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="G12">
-        <v>4.0999999999999996</v>
+        <v>41</v>
       </c>
       <c r="H12">
-        <v>6.1</v>
+        <v>61</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>